<commit_message>
Final push of SHL GenAI: cleaned .gitignore, code, docs, artifacts.
</commit_message>
<xml_diff>
--- a/data/Gen_AI Dataset.xlsx
+++ b/data/Gen_AI Dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnav.Gupta\Downloads\Intern Hiring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SHL Internship\projects\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{E3E4D141-5E23-457A-B881-52BE38519C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D442DBE2-A0CF-491B-837A-4A76A1E03A5E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94469F72-14B7-4F6F-A566-84D3C5BFCBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{25D3A309-194C-4227-8A23-86D8595035ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{25D3A309-194C-4227-8A23-86D8595035ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Train-Set" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -571,7 +560,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -973,17 +962,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4AB23EC-048F-4FC6-8065-B84C5D0C6832}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="145.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="145.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -991,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -999,7 +988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1015,7 +1004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1023,7 +1012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1031,7 +1020,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1039,7 +1028,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1047,7 +1036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1055,7 +1044,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +1052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1071,7 +1060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1079,7 +1068,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1087,7 +1076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1095,7 +1084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1103,7 +1092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1111,7 +1100,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1119,7 +1108,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1127,7 +1116,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1135,7 +1124,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1143,7 +1132,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1151,7 +1140,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1159,7 +1148,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1167,7 +1156,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1175,7 +1164,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1183,7 +1172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1191,7 +1180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1199,7 +1188,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1207,7 +1196,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1215,7 +1204,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1223,7 +1212,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1231,7 +1220,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1239,7 +1228,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1247,7 +1236,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1255,7 +1244,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1263,7 +1252,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1271,7 +1260,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1279,7 +1268,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -1287,7 +1276,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -1295,7 +1284,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1303,7 +1292,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -1311,7 +1300,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -1319,7 +1308,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1327,7 +1316,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1335,7 +1324,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1343,7 +1332,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1351,7 +1340,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -1359,7 +1348,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -1367,7 +1356,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -1375,7 +1364,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1383,7 +1372,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1391,7 +1380,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1399,7 +1388,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -1407,7 +1396,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -1415,7 +1404,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -1423,7 +1412,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -1431,7 +1420,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -1439,7 +1428,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -1447,7 +1436,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -1455,7 +1444,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1463,7 +1452,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1471,7 +1460,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -1479,7 +1468,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -1487,7 +1476,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>59</v>
       </c>
@@ -1495,7 +1484,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>59</v>
       </c>
@@ -1503,7 +1492,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>59</v>
       </c>
@@ -1545,58 +1534,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004DCD8D-393B-403B-9024-9664EA271AB7}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="74" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>74</v>
       </c>

</xml_diff>